<commit_message>
corrected numbering in readme
</commit_message>
<xml_diff>
--- a/demographics for business plan.xlsx
+++ b/demographics for business plan.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <fileSharing readOnlyRecommended="1" userName="Andrea" algorithmName="SHA-512" hashValue="wFnbioHiyEepzNGEgpcNmweTMJo52n4EwQxcIjF5t630Go3W1t5Cc2KMyxm/iWuu9n/i+QY8vc2TUNGjp78XBA==" saltValue="NaDkin0r+pLFMRLHlVqOHw==" spinCount="100000"/>
+  <fileSharing userName="Andrea" algorithmName="SHA-512" hashValue="6WWJsBK0WjuLxJjwtLUd01gJ4HPW8eRkTzctlvhaG4WQ4TZpNjyssERF9xEX2QUXa/1yVMmExC6EVtuUyRgCnA==" saltValue="luLJQ7Zv4/+28viqa1xsHw==" spinCount="100000"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,13 +10,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11355" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11355"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
     <sheet name="properties" sheetId="1" r:id="rId2"/>
     <sheet name="Final Summary" sheetId="5" r:id="rId3"/>
-    <sheet name="ESRI data" sheetId="3" r:id="rId4"/>
+    <sheet name="ESRI data" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ESRI data'!$A$1:$S$33</definedName>
@@ -25,8 +25,8 @@
     <definedName name="_xlchart.0" hidden="1">properties!$AP$2</definedName>
     <definedName name="_xlchart.1" hidden="1">properties!$AP$3:$AP$34</definedName>
     <definedName name="_xlchart.2" hidden="1">properties!$C$3:$C$34</definedName>
-    <definedName name="_xlcn.WorksheetConnection_ESRIdataA1R33" hidden="1">'ESRI data'!$A$1:$R$33</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Sheet1A1EP33" hidden="1">properties!$A$2:$FE$34</definedName>
+    <definedName name="_xlcn.WorksheetConnection_ESRIdataA1R331" hidden="1">'ESRI data'!$A$1:$R$33</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Sheet1A1EP331" hidden="1">properties!$A$2:$FE$34</definedName>
     <definedName name="Z_76F2D8D9_A5B3_4AF2_A9E6_D7B3EADB6426_.wvu.Cols" localSheetId="1" hidden="1">properties!$A:$A,properties!$O:$FE</definedName>
     <definedName name="Z_7BEC8753_17A4_4365_A266_EAB72C4F1E8D_.wvu.Cols" localSheetId="1" hidden="1">properties!$A:$B</definedName>
     <definedName name="Z_89E3B238_0CC8_42EF_8051_0391F72923CF_.wvu.Cols" localSheetId="1" hidden="1">properties!$A:$B,properties!$F:$J,properties!$M:$M,properties!$P:$Q,properties!$T:$U,properties!$W:$Y,properties!$AB:$AC,properties!$AE:$AF,properties!$AH:$EL,properties!$EO:$FE</definedName>
@@ -170,7 +170,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_ESRIdataA1R33"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_ESRIdataA1R331"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -179,7 +179,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1A1EP33"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1A1EP331"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1638,6 +1638,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2302,6 +2303,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2383,6 +2385,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2482,6 +2485,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4186,6 +4190,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4828,6 +4833,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16182,8 +16188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16203,10 +16209,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FT65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="FE2" sqref="C2:FE2"/>
+      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38298,9 +38304,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -38310,7 +38315,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>